<commit_message>
Added division and address supplement
</commit_message>
<xml_diff>
--- a/appdata/static/export/export.xlsx
+++ b/appdata/static/export/export.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\mailing\appdata\static\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024DAAE2-F4D5-4E17-A57A-0BBE5B1E899D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8226E0CD-99CD-4296-8F05-FE9FBC86EF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22597" yWindow="-4125" windowWidth="22695" windowHeight="14595" xr2:uid="{F2DD96FB-E7EA-49CD-A96C-71A5E17901E1}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F2DD96FB-E7EA-49CD-A96C-71A5E17901E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Fachhändler</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Nachname</t>
+  </si>
+  <si>
+    <t>Abteilung</t>
+  </si>
+  <si>
+    <t>Adresszusatz</t>
   </si>
 </sst>
 </file>
@@ -455,21 +461,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41A68AA-E914-4A84-9251-B8681C0E9C44}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -510,33 +517,39 @@
         <v>9</v>
       </c>
       <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>19</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>